<commit_message>
Start supporting localized messages
</commit_message>
<xml_diff>
--- a/inc/messages/messages.xlsx
+++ b/inc/messages/messages.xlsx
@@ -2324,8 +2324,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:B335"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="A231" sqref="A231:XFD231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.9"/>

</xml_diff>